<commit_message>
putting overall on the spreadsheet
</commit_message>
<xml_diff>
--- a/players_atributes.xlsx
+++ b/players_atributes.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -27,6 +27,7 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
@@ -40,7 +41,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFffff00"/>
       </patternFill>
     </fill>
   </fills>
@@ -76,7 +77,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -158,10 +161,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -199,71 +202,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -291,7 +294,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -314,11 +317,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -327,13 +330,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -343,7 +346,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -352,7 +355,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -361,7 +364,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -369,10 +372,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -442,19 +445,25 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="18.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="16.85546875" customWidth="1" style="2" min="1" max="1"/>
-    <col width="18.5703125" customWidth="1" style="2" min="2" max="7"/>
+    <col width="16.86214285714286" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="18.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="18.57642857142857" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="18.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
+    <col width="18.57642857142857" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
+    <col width="18.57642857142857" bestFit="1" customWidth="1" style="2" min="6" max="6"/>
+    <col width="18.57642857142857" bestFit="1" customWidth="1" style="2" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" customHeight="1" s="2">
+    <row r="1" ht="20.25" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Nome</t>
@@ -488,81 +497,42 @@
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>CRE</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>OVERALL</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Wagner Junior</t>
+          <t>Lionel Messi</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MC</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>85</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>57</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>92</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Lionel Messi</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
           <t>PD</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>99</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>98</t>
-        </is>
+      <c r="C2" t="n">
+        <v>98</v>
+      </c>
+      <c r="D2" t="n">
+        <v>97</v>
+      </c>
+      <c r="E2" t="n">
+        <v>58</v>
+      </c>
+      <c r="F2" t="n">
+        <v>40</v>
+      </c>
+      <c r="G2" t="n">
+        <v>99</v>
+      </c>
+      <c r="H2" t="n">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>